<commit_message>
More progress. Geocoded stadiums.
More progress. Geocoded stadiums.
</commit_message>
<xml_diff>
--- a/RWC2023Pools.xlsx
+++ b/RWC2023Pools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts_mc\Code\Github\Pandas_Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24A8C0E-E582-466A-843D-CD5C2B383022}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C68A2C1-3004-4B26-98F4-7FA84A3DEAEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="18224" windowHeight="10957" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="1245" windowWidth="18225" windowHeight="10957" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PoolA" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -635,10 +635,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1005,8 +1005,8 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1102,22 +1102,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>45183</v>
+        <v>45178</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
         <v>41</v>
@@ -1128,22 +1128,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>45184</v>
+        <v>45178</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -1154,22 +1154,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>45189</v>
+        <v>45178</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
         <v>41</v>
@@ -1180,19 +1180,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>45190</v>
+        <v>45179</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -1206,22 +1206,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>45196</v>
+        <v>45179</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
         <v>41</v>
@@ -1232,22 +1232,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>45198</v>
+        <v>45179</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
         <v>41</v>
@@ -1261,19 +1261,19 @@
         <v>36</v>
       </c>
       <c r="C10" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>45204</v>
+        <v>45183</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
         <v>41</v>
@@ -1287,19 +1287,19 @@
         <v>36</v>
       </c>
       <c r="C11" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D11" s="3">
-        <v>45205</v>
+        <v>45184</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
         <v>41</v>
@@ -1313,19 +1313,19 @@
         <v>37</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>45178</v>
+        <v>45185</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
         <v>41</v>
@@ -1336,22 +1336,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="3">
-        <v>45179</v>
+        <v>45185</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
@@ -1362,7 +1362,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5">
         <v>2</v>
@@ -1371,13 +1371,13 @@
         <v>45185</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -1414,22 +1414,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3">
-        <v>45192</v>
+        <v>45186</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
         <v>41</v>
@@ -1440,19 +1440,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17" s="3">
-        <v>45193</v>
+        <v>45186</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>9</v>
@@ -1466,22 +1466,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45189</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="3">
-        <v>45199</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H18" t="s">
         <v>41</v>
@@ -1492,19 +1492,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3">
-        <v>45200</v>
+        <v>45190</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
@@ -1518,22 +1518,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D20" s="3">
-        <v>45206</v>
+        <v>45191</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
         <v>41</v>
@@ -1547,19 +1547,19 @@
         <v>37</v>
       </c>
       <c r="C21" s="5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D21" s="3">
-        <v>45207</v>
+        <v>45192</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H21" t="s">
         <v>41</v>
@@ -1573,19 +1573,19 @@
         <v>38</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22" s="3">
-        <v>45178</v>
+        <v>45192</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
         <v>41</v>
@@ -1596,22 +1596,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D23" s="3">
-        <v>45179</v>
+        <v>45192</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
         <v>41</v>
@@ -1622,19 +1622,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D24" s="3">
-        <v>45185</v>
+        <v>45193</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -1651,19 +1651,19 @@
         <v>38</v>
       </c>
       <c r="C25" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3">
-        <v>45186</v>
+        <v>45193</v>
       </c>
       <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" t="s">
-        <v>28</v>
-      </c>
       <c r="G25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
         <v>41</v>
@@ -1674,22 +1674,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="5">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45196</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="3">
-        <v>45192</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
-        <v>29</v>
-      </c>
       <c r="G26" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
         <v>41</v>
@@ -1700,22 +1700,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" s="3">
-        <v>45193</v>
+        <v>45197</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
         <v>41</v>
@@ -1726,22 +1726,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3">
-        <v>45199</v>
+        <v>45198</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H28" t="s">
         <v>41</v>
@@ -1752,22 +1752,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="5">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45199</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
         <v>7</v>
-      </c>
-      <c r="D29" s="3">
-        <v>45200</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" t="s">
-        <v>5</v>
       </c>
       <c r="H29" t="s">
         <v>41</v>
@@ -1781,19 +1781,19 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30" s="3">
-        <v>45206</v>
+        <v>45199</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F30" t="s">
         <v>26</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H30" t="s">
         <v>41</v>
@@ -1804,22 +1804,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D31" s="3">
-        <v>45207</v>
+        <v>45199</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H31" t="s">
         <v>41</v>
@@ -1830,19 +1830,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D32" s="3">
-        <v>45178</v>
+        <v>45200</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G32" t="s">
         <v>10</v>
@@ -1856,22 +1856,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D33" s="3">
-        <v>45179</v>
+        <v>45200</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H33" t="s">
         <v>41</v>
@@ -1882,22 +1882,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C34" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D34" s="3">
-        <v>45185</v>
+        <v>45204</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H34" t="s">
         <v>41</v>
@@ -1908,22 +1908,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35" s="5">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45205</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="3">
-        <v>45186</v>
-      </c>
-      <c r="E35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" t="s">
-        <v>32</v>
-      </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H35" t="s">
         <v>41</v>
@@ -1934,22 +1934,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36" s="3">
-        <v>45191</v>
+        <v>45206</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F36" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
         <v>41</v>
@@ -1960,22 +1960,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D37" s="3">
-        <v>45192</v>
+        <v>45206</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="H37" t="s">
         <v>41</v>
@@ -1989,19 +1989,19 @@
         <v>39</v>
       </c>
       <c r="C38" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D38" s="3">
-        <v>45197</v>
+        <v>45206</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s">
         <v>41</v>
@@ -2012,22 +2012,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" s="5">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45207</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" t="s">
         <v>7</v>
-      </c>
-      <c r="D39" s="3">
-        <v>45199</v>
-      </c>
-      <c r="E39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" t="s">
-        <v>24</v>
       </c>
       <c r="H39" t="s">
         <v>41</v>
@@ -2038,22 +2038,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45207</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" t="s">
         <v>8</v>
-      </c>
-      <c r="D40" s="3">
-        <v>45206</v>
-      </c>
-      <c r="E40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" t="s">
-        <v>7</v>
       </c>
       <c r="H40" t="s">
         <v>41</v>
@@ -2086,6 +2086,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
+    <sortCondition ref="D2:D42"/>
+    <sortCondition ref="B2:B42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>